<commit_message>
Remove some constants, add some error catches
</commit_message>
<xml_diff>
--- a/test file.xlsx
+++ b/test file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KEVIN PHAM\Documents\GitHub\genasys-test-viewer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CE0D7A-F627-47DE-AE95-5B203F01CBA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D679F31E-7753-4695-AA74-D953A95F60CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,9 +27,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
-    <t>UNIT SN</t>
-  </si>
-  <si>
     <t>Date</t>
   </si>
   <si>
@@ -43,6 +40,9 @@
   </si>
   <si>
     <t>PASSED</t>
+  </si>
+  <si>
+    <t>Unit SN</t>
   </si>
 </sst>
 </file>
@@ -374,7 +374,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,16 +385,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -408,7 +408,7 @@
         <v>0.69027777777777777</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -433,7 +433,7 @@
         <v>0.71805555555555556</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -447,7 +447,7 @@
         <v>0.87569444444444444</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>